<commit_message>
Added 2023 NFL Conference Championship Forecasts
</commit_message>
<xml_diff>
--- a/seasons/AmericanFootball/NationalFootballLeague/2023/forecasts/matrix_DIV.xlsx
+++ b/seasons/AmericanFootball/NationalFootballLeague/2023/forecasts/matrix_DIV.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,16 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\SportPredictifier\SportPredictifier\seasons\AmericanFootball\NationalFootballLeague\2023\forecasts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{68B6DC9C-8789-464D-AD4A-2DAE73F4635C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF47311-5690-46F5-B6B7-0FCB333F14E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projected Bracket" sheetId="4" r:id="rId1"/>
     <sheet name="matrix_DIV" sheetId="1" r:id="rId2"/>
     <sheet name="Forecasts" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -44,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="53">
   <si>
     <t>BAL</t>
   </si>
@@ -208,7 +221,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#0"/>
     <numFmt numFmtId="165" formatCode="#0%"/>
@@ -1050,7 +1063,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1093,8 +1106,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1104,9 +1118,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1133,30 +1144,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="47" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="47" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="47" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="47" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1258,7 +1245,7 @@
     <xf numFmtId="0" fontId="0" fillId="49" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="49" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="49" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1285,8 +1272,36 @@
     <xf numFmtId="0" fontId="0" fillId="49" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="47" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="47" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="47" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="47" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1326,6 +1341,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -1665,540 +1681,540 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="13"/>
-    <col min="2" max="2" width="3.33203125" style="13" customWidth="1"/>
-    <col min="3" max="4" width="5.77734375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="3.33203125" style="13" customWidth="1"/>
-    <col min="6" max="7" width="5.77734375" style="13" customWidth="1"/>
-    <col min="8" max="8" width="3.33203125" style="13" customWidth="1"/>
-    <col min="9" max="10" width="5.77734375" style="13" customWidth="1"/>
-    <col min="11" max="12" width="7.77734375" style="13" customWidth="1"/>
-    <col min="13" max="14" width="5.77734375" style="13" customWidth="1"/>
-    <col min="15" max="15" width="3.33203125" style="13" customWidth="1"/>
-    <col min="16" max="17" width="5.77734375" style="13" customWidth="1"/>
-    <col min="18" max="18" width="3.33203125" style="13" customWidth="1"/>
-    <col min="19" max="20" width="5.77734375" style="13" customWidth="1"/>
-    <col min="21" max="21" width="3.33203125" style="13" customWidth="1"/>
-    <col min="22" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="1" width="8.88671875" style="12"/>
+    <col min="2" max="2" width="3.33203125" style="12" customWidth="1"/>
+    <col min="3" max="4" width="5.77734375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="3.33203125" style="12" customWidth="1"/>
+    <col min="6" max="7" width="5.77734375" style="12" customWidth="1"/>
+    <col min="8" max="8" width="3.33203125" style="12" customWidth="1"/>
+    <col min="9" max="10" width="5.77734375" style="12" customWidth="1"/>
+    <col min="11" max="12" width="7.77734375" style="12" customWidth="1"/>
+    <col min="13" max="14" width="5.77734375" style="12" customWidth="1"/>
+    <col min="15" max="15" width="3.33203125" style="12" customWidth="1"/>
+    <col min="16" max="17" width="5.77734375" style="12" customWidth="1"/>
+    <col min="18" max="18" width="3.33203125" style="12" customWidth="1"/>
+    <col min="19" max="20" width="5.77734375" style="12" customWidth="1"/>
+    <col min="21" max="21" width="3.33203125" style="12" customWidth="1"/>
+    <col min="22" max="16384" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="52"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="58"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="49"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="18" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="19"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="55"/>
-      <c r="U3" s="59"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="50"/>
     </row>
     <row r="4" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="20" t="s">
+      <c r="B4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="21"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="55"/>
-      <c r="S4" s="55"/>
-      <c r="T4" s="55"/>
-      <c r="U4" s="59"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="46"/>
+      <c r="T4" s="46"/>
+      <c r="U4" s="50"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="14" t="s">
+      <c r="B5" s="45"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="15"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="55"/>
-      <c r="R5" s="55"/>
-      <c r="S5" s="55"/>
-      <c r="T5" s="55"/>
-      <c r="U5" s="59"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="50"/>
     </row>
     <row r="6" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="16" t="s">
+      <c r="B6" s="45"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="55"/>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="55"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="55"/>
-      <c r="U6" s="59"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="50"/>
     </row>
     <row r="7" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="54"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="55"/>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="55"/>
-      <c r="S7" s="55"/>
-      <c r="T7" s="55"/>
-      <c r="U7" s="59"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="50"/>
     </row>
     <row r="8" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="26" t="s">
+      <c r="B8" s="45"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="56"/>
-      <c r="N8" s="55"/>
-      <c r="O8" s="55"/>
-      <c r="P8" s="55"/>
-      <c r="Q8" s="55"/>
-      <c r="R8" s="55"/>
-      <c r="S8" s="55"/>
-      <c r="T8" s="55"/>
-      <c r="U8" s="59"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="46"/>
+      <c r="U8" s="50"/>
     </row>
     <row r="9" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="22">
+      <c r="B9" s="45"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="13">
         <v>23.761296999999999</v>
       </c>
-      <c r="L9" s="23">
+      <c r="L9" s="14">
         <v>22.948779999999999</v>
       </c>
-      <c r="M9" s="57"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="59"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="50"/>
     </row>
     <row r="10" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="57"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="55"/>
-      <c r="R10" s="55"/>
-      <c r="S10" s="55"/>
-      <c r="T10" s="55"/>
-      <c r="U10" s="59"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="46"/>
+      <c r="U10" s="50"/>
     </row>
     <row r="11" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="28" t="s">
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="30" t="s">
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N11" s="31" t="s">
+      <c r="N11" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="O11" s="55"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="55"/>
-      <c r="R11" s="55"/>
-      <c r="S11" s="55"/>
-      <c r="T11" s="55"/>
-      <c r="U11" s="59"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="46"/>
+      <c r="S11" s="46"/>
+      <c r="T11" s="46"/>
+      <c r="U11" s="50"/>
     </row>
     <row r="12" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="24">
+      <c r="B12" s="45"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="15">
         <v>24.115272999999998</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="16">
         <v>21.052873000000002</v>
       </c>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="22">
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="13">
         <v>29.334658000000001</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="14">
         <v>23.435181</v>
       </c>
-      <c r="O12" s="55"/>
-      <c r="P12" s="55"/>
-      <c r="Q12" s="55"/>
-      <c r="R12" s="55"/>
-      <c r="S12" s="55"/>
-      <c r="T12" s="55"/>
-      <c r="U12" s="59"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="46"/>
+      <c r="S12" s="46"/>
+      <c r="T12" s="46"/>
+      <c r="U12" s="50"/>
     </row>
     <row r="13" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="54"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="55"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="55"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="59"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="46"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="46"/>
+      <c r="S13" s="46"/>
+      <c r="T13" s="46"/>
+      <c r="U13" s="50"/>
     </row>
     <row r="14" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="32" t="s">
+      <c r="B14" s="45"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="56"/>
-      <c r="I14" s="28" t="s">
+      <c r="H14" s="47"/>
+      <c r="I14" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="J14" s="34" t="s">
+      <c r="J14" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="40" t="s">
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="N14" s="41" t="s">
+      <c r="N14" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="O14" s="56"/>
-      <c r="P14" s="42" t="s">
+      <c r="O14" s="47"/>
+      <c r="P14" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="Q14" s="43" t="s">
+      <c r="Q14" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="R14" s="56"/>
-      <c r="S14" s="56"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="59"/>
+      <c r="R14" s="47"/>
+      <c r="S14" s="47"/>
+      <c r="T14" s="46"/>
+      <c r="U14" s="50"/>
     </row>
     <row r="15" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="54"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="24">
+      <c r="B15" s="45"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="15">
         <v>21.468913000000001</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="16">
         <v>18.514786999999998</v>
       </c>
-      <c r="H15" s="55"/>
-      <c r="I15" s="24">
+      <c r="H15" s="46"/>
+      <c r="I15" s="15">
         <v>27.939754000000001</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15" s="16">
         <v>16.984933000000002</v>
       </c>
-      <c r="K15" s="55"/>
-      <c r="L15" s="55"/>
-      <c r="M15" s="24">
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="15">
         <v>27.263814</v>
       </c>
-      <c r="N15" s="25">
+      <c r="N15" s="16">
         <v>20.307295</v>
       </c>
-      <c r="O15" s="55"/>
-      <c r="P15" s="24">
+      <c r="O15" s="46"/>
+      <c r="P15" s="15">
         <v>24.29663</v>
       </c>
-      <c r="Q15" s="25">
+      <c r="Q15" s="16">
         <v>21.819742999999999</v>
       </c>
-      <c r="R15" s="55"/>
-      <c r="S15" s="57"/>
-      <c r="T15" s="55"/>
-      <c r="U15" s="59"/>
+      <c r="R15" s="46"/>
+      <c r="S15" s="48"/>
+      <c r="T15" s="46"/>
+      <c r="U15" s="50"/>
     </row>
     <row r="16" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="54"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="55"/>
-      <c r="R16" s="55"/>
-      <c r="S16" s="57"/>
-      <c r="T16" s="55"/>
-      <c r="U16" s="59"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="46"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="46"/>
+      <c r="U16" s="50"/>
     </row>
     <row r="17" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="54"/>
-      <c r="C17" s="32" t="s">
+      <c r="B17" s="45"/>
+      <c r="C17" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="55"/>
-      <c r="F17" s="36" t="s">
+      <c r="E17" s="46"/>
+      <c r="F17" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="H17" s="55"/>
-      <c r="I17" s="38" t="s">
+      <c r="H17" s="46"/>
+      <c r="I17" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="39" t="s">
+      <c r="J17" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="55"/>
-      <c r="L17" s="55"/>
-      <c r="M17" s="44" t="s">
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="N17" s="41" t="s">
+      <c r="N17" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="O17" s="55"/>
-      <c r="P17" s="42" t="s">
+      <c r="O17" s="46"/>
+      <c r="P17" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="Q17" s="45" t="s">
+      <c r="Q17" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="55"/>
-      <c r="S17" s="46" t="s">
+      <c r="R17" s="46"/>
+      <c r="S17" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="T17" s="47" t="s">
+      <c r="T17" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="U17" s="59"/>
+      <c r="U17" s="50"/>
     </row>
     <row r="18" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="54"/>
-      <c r="C18" s="48">
+      <c r="B18" s="45"/>
+      <c r="C18" s="39">
         <v>31</v>
       </c>
-      <c r="D18" s="49">
-        <v>17</v>
-      </c>
-      <c r="E18" s="55"/>
-      <c r="F18" s="48">
+      <c r="D18" s="40">
+        <v>17</v>
+      </c>
+      <c r="E18" s="46"/>
+      <c r="F18" s="39">
         <v>26</v>
       </c>
-      <c r="G18" s="49">
+      <c r="G18" s="40">
         <v>7</v>
       </c>
-      <c r="H18" s="55"/>
-      <c r="I18" s="48">
+      <c r="H18" s="46"/>
+      <c r="I18" s="39">
         <v>45</v>
       </c>
-      <c r="J18" s="49">
+      <c r="J18" s="40">
         <v>14</v>
       </c>
-      <c r="K18" s="55"/>
-      <c r="L18" s="55"/>
-      <c r="M18" s="50">
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="41">
         <v>32</v>
       </c>
-      <c r="N18" s="51">
+      <c r="N18" s="42">
         <v>48</v>
       </c>
-      <c r="O18" s="55"/>
-      <c r="P18" s="48">
-        <v>24</v>
-      </c>
-      <c r="Q18" s="49">
+      <c r="O18" s="46"/>
+      <c r="P18" s="39">
+        <v>24</v>
+      </c>
+      <c r="Q18" s="40">
         <v>23</v>
       </c>
-      <c r="R18" s="55"/>
-      <c r="S18" s="48">
+      <c r="R18" s="46"/>
+      <c r="S18" s="39">
         <v>32</v>
       </c>
-      <c r="T18" s="49">
+      <c r="T18" s="40">
         <v>9</v>
       </c>
-      <c r="U18" s="59"/>
+      <c r="U18" s="50"/>
     </row>
     <row r="19" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="63"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="61"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="61"/>
-      <c r="P19" s="61"/>
-      <c r="Q19" s="61"/>
-      <c r="R19" s="61"/>
-      <c r="S19" s="61"/>
-      <c r="T19" s="61"/>
-      <c r="U19" s="62"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="52"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="52"/>
+      <c r="T19" s="52"/>
+      <c r="U19" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2213,11 +2229,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2483,6 +2499,12 @@
         <f t="array" ref="D12">C12*MMULT(F2:I2, $C$16:$C$19)</f>
         <v>0.35734273354454144</v>
       </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="64">
+        <v>0.35734273354454144</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -2500,6 +2522,12 @@
         <f t="array" ref="D13">C13*MMULT(F3:I3, $C$16:$C$19)</f>
         <v>0.14384613702088947</v>
       </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="64">
+        <v>0.31850519428703439</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -2517,6 +2545,12 @@
         <f t="array" ref="D14">C14*MMULT(F4:I4, $C$16:$C$19)</f>
         <v>4.6666316239802517E-2</v>
       </c>
+      <c r="F14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="64">
+        <v>0.14384613702088947</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -2534,6 +2568,12 @@
         <f t="array" ref="D15">C15*MMULT(F5:I5, $C$16:$C$19)</f>
         <v>8.2713592662329027E-3</v>
       </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="64">
+        <v>6.7321354326519506E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -2551,8 +2591,14 @@
         <f t="array" ref="D16">C16*MMULT(B6:E6, $C$12:$C$15)</f>
         <v>0.31850519428703439</v>
       </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="64">
+        <v>4.6666316239802517E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -2568,8 +2614,14 @@
         <f t="array" ref="D17">C17*MMULT(B7:E7, $C$12:$C$15)</f>
         <v>6.7321354326519506E-2</v>
       </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="64">
+        <v>3.3701444530866542E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -2585,8 +2637,14 @@
         <f t="array" ref="D18">C18*MMULT(B8:E8, $C$12:$C$15)</f>
         <v>2.4345460784113308E-2</v>
       </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="64">
+        <v>2.4345460784113308E-2</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2602,14 +2660,23 @@
         <f t="array" ref="D19">C19*MMULT(B9:E9, $C$12:$C$15)</f>
         <v>3.3701444530866542E-2</v>
       </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="64">
+        <v>8.2713592662329027E-3</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F12:G19">
+    <sortCondition descending="1" ref="G12:G19"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CF26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2679,172 +2746,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:84" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AA1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AF1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AG1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AI1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AJ1" s="11" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AL1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AM1" s="12" t="s">
+      <c r="AM1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AO1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AP1" s="12" t="s">
+      <c r="AP1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AR1" s="7" t="s">
+      <c r="AR1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AS1" s="8" t="s">
+      <c r="AS1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AU1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AV1" s="12" t="s">
+      <c r="AV1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AX1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AY1" s="7" t="s">
+      <c r="AY1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BA1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BB1" s="10" t="s">
+      <c r="BB1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="BD1" s="12" t="s">
+      <c r="BD1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BE1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BG1" s="11" t="s">
+      <c r="BG1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="BH1" s="5" t="s">
+      <c r="BH1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BJ1" s="11" t="s">
+      <c r="BJ1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="BK1" s="12" t="s">
+      <c r="BK1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="BM1" s="6" t="s">
+      <c r="BM1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="BN1" s="11" t="s">
+      <c r="BN1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="BP1" s="6" t="s">
+      <c r="BP1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="BQ1" s="10" t="s">
+      <c r="BQ1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="BS1" s="8" t="s">
+      <c r="BS1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="BT1" s="5" t="s">
+      <c r="BT1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BV1" s="9" t="s">
+      <c r="BV1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="BW1" s="5" t="s">
+      <c r="BW1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BY1" s="6" t="s">
+      <c r="BY1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="BZ1" s="8" t="s">
+      <c r="BZ1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="CB1" s="7" t="s">
+      <c r="CB1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="CC1" s="5" t="s">
+      <c r="CC1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CE1" s="6" t="s">
+      <c r="CE1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="CF1" s="5" t="s">
+      <c r="CF1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2852,118 +2919,118 @@
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="F2" s="63"/>
+      <c r="H2" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="I2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="N2" s="4" t="s">
+      <c r="L2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="Q2" s="4" t="s">
+      <c r="O2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="4"/>
-      <c r="T2" s="4" t="s">
+      <c r="R2" s="63"/>
+      <c r="T2" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="W2" s="4" t="s">
+      <c r="U2" s="63"/>
+      <c r="W2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="X2" s="4"/>
-      <c r="Z2" s="4" t="s">
+      <c r="X2" s="63"/>
+      <c r="Z2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="AA2" s="4"/>
-      <c r="AC2" s="4" t="s">
+      <c r="AA2" s="63"/>
+      <c r="AC2" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="AD2" s="4"/>
-      <c r="AF2" s="4" t="s">
+      <c r="AD2" s="63"/>
+      <c r="AF2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="AG2" s="4"/>
-      <c r="AI2" s="4" t="s">
+      <c r="AG2" s="63"/>
+      <c r="AI2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="AJ2" s="4"/>
-      <c r="AL2" s="4" t="s">
+      <c r="AJ2" s="63"/>
+      <c r="AL2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="AM2" s="4"/>
-      <c r="AO2" s="4" t="s">
+      <c r="AM2" s="63"/>
+      <c r="AO2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="AP2" s="4"/>
-      <c r="AR2" s="4" t="s">
+      <c r="AP2" s="63"/>
+      <c r="AR2" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="AS2" s="4"/>
-      <c r="AU2" s="4" t="s">
+      <c r="AS2" s="63"/>
+      <c r="AU2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="AV2" s="4"/>
-      <c r="AX2" s="4" t="s">
+      <c r="AV2" s="63"/>
+      <c r="AX2" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="AY2" s="4"/>
-      <c r="BA2" s="4" t="s">
+      <c r="AY2" s="63"/>
+      <c r="BA2" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="BB2" s="4"/>
-      <c r="BD2" s="4" t="s">
+      <c r="BB2" s="63"/>
+      <c r="BD2" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="BE2" s="4"/>
-      <c r="BG2" s="4" t="s">
+      <c r="BE2" s="63"/>
+      <c r="BG2" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="BH2" s="4"/>
-      <c r="BJ2" s="4" t="s">
+      <c r="BH2" s="63"/>
+      <c r="BJ2" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="BK2" s="4"/>
-      <c r="BM2" s="4" t="s">
+      <c r="BK2" s="63"/>
+      <c r="BM2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="BN2" s="4"/>
-      <c r="BP2" s="4" t="s">
+      <c r="BN2" s="63"/>
+      <c r="BP2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="BQ2" s="4"/>
-      <c r="BS2" s="4" t="s">
+      <c r="BQ2" s="63"/>
+      <c r="BS2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="BT2" s="4"/>
-      <c r="BV2" s="4" t="s">
+      <c r="BT2" s="63"/>
+      <c r="BV2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="BW2" s="4"/>
-      <c r="BY2" s="4" t="s">
+      <c r="BW2" s="63"/>
+      <c r="BY2" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="BZ2" s="4"/>
-      <c r="CB2" s="4" t="s">
+      <c r="BZ2" s="63"/>
+      <c r="CB2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="CC2" s="4"/>
-      <c r="CE2" s="4" t="s">
+      <c r="CC2" s="63"/>
+      <c r="CE2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="CF2" s="4"/>
+      <c r="CF2" s="63"/>
     </row>
     <row r="3" spans="1:84" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -6615,26 +6682,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="BA2:BB2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BG2:BH2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AR2:AS2"/>
     <mergeCell ref="BY2:BZ2"/>
     <mergeCell ref="CB2:CC2"/>
     <mergeCell ref="CE2:CF2"/>
@@ -6643,6 +6690,26 @@
     <mergeCell ref="BP2:BQ2"/>
     <mergeCell ref="BS2:BT2"/>
     <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="BA2:BB2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BG2:BH2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AC2:AD2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>